<commit_message>
Add duplicatie entries validation on user import
</commit_message>
<xml_diff>
--- a/user.xlsx
+++ b/user.xlsx
@@ -110,7 +110,7 @@
     <t>2nd</t>
   </si>
   <si>
-    <t>user_year (1st, 2nd, 3rd, 4th, Terminal)</t>
+    <t>user_year</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Duplicate Validation on Import
</commit_message>
<xml_diff>
--- a/user.xlsx
+++ b/user.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>user_number</t>
   </si>
@@ -68,27 +68,15 @@
     <t>Two</t>
   </si>
   <si>
-    <t>Three</t>
-  </si>
-  <si>
     <t>BSITAGD</t>
   </si>
   <si>
-    <t>BSITDA</t>
-  </si>
-  <si>
     <t>be9f57a7bbea5f7489e601db0cecffcfdd91e507</t>
   </si>
   <si>
-    <t>e1167ee6d7e042ce7e223584fa6b44a5c2d92b51</t>
-  </si>
-  <si>
     <t>tdc@fit.edu.ph</t>
   </si>
   <si>
-    <t>thdc@fit.edu.ph</t>
-  </si>
-  <si>
     <t>user_section</t>
   </si>
   <si>
@@ -104,13 +92,13 @@
     <t>Terminal</t>
   </si>
   <si>
-    <t>A41</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
     <t>user_year</t>
+  </si>
+  <si>
+    <t>be9f57a7bbea5f7489e601db0cecffcfdd91e508</t>
+  </si>
+  <si>
+    <t>X42</t>
   </si>
 </sst>
 </file>
@@ -441,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,15 +465,15 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>201500001</v>
+        <v>201500005</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -506,15 +494,15 @@
         <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>201500002</v>
+        <v>201500006</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -526,27 +514,27 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>201500003</v>
+        <v>201500005</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -555,26 +543,86 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>201500006</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>201500007</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>27</v>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>